<commit_message>
Wip Checklist Adds files in order to read menu and payments
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Anul3Sem2\ValidareaVerificareaSistemlorSoft\Labs\Grupul_Angajatilor_Young\Docs\Lab1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF0857B-6229-4E9A-A31C-D041BE9229D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="14160" windowHeight="8268" tabRatio="650"/>
+    <workbookView xWindow="0" yWindow="852" windowWidth="23004" windowHeight="11508" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -12,12 +18,25 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="45">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -116,19 +135,62 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours):</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>R05</t>
+  </si>
+  <si>
+    <t>R06</t>
+  </si>
+  <si>
+    <t>R07</t>
+  </si>
+  <si>
+    <t>Ce se intampla daca cele 8 mese sunt ocupate? - Mesaj de informare</t>
+  </si>
+  <si>
+    <t>Meniul se incarca doar la pornirea aplicatiei? - da</t>
+  </si>
+  <si>
+    <t>De cate aplicatii este nevoie? Client, Chelner, Bucatar?</t>
+  </si>
+  <si>
+    <t>Butacu Stefan</t>
+  </si>
+  <si>
+    <t>Cadar Eduard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -198,6 +260,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -302,77 +371,77 @@
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,6 +451,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -430,7 +502,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -463,9 +535,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -498,6 +587,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -673,105 +779,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.41796875" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.89453125" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="14" t="s">
+      <c r="I3" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="17">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="25"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="24"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="14" t="s">
+      <c r="I4" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="26"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -781,73 +895,93 @@
       <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E16" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -856,86 +990,83 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="16"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E18" s="15"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="1"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="16"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E19" s="15"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="1"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="16"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E20" s="15"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="3"/>
+      <c r="C21" s="1"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="16"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="16"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="12" t="s">
+      <c r="E25" s="15"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="13"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="1"/>
     </row>
   </sheetData>
@@ -947,110 +1078,111 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D5:E5"/>
   </mergeCells>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.3125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="22.05078125" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="22" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="27"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="29"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1064,7 +1196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1072,7 +1204,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1081,7 +1213,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -1090,7 +1222,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1099,7 +1231,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1108,7 +1240,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1117,7 +1249,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1126,7 +1258,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1135,7 +1267,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1144,7 +1276,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1153,7 +1285,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1162,7 +1294,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1171,7 +1303,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1180,7 +1312,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1189,7 +1321,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1198,7 +1330,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1207,7 +1339,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1216,14 +1348,11 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="12" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="13"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="1"/>
     </row>
   </sheetData>
@@ -1241,7 +1370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1251,95 +1380,95 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="41.41796875" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="41.44140625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="H4" s="18" t="s">
+      <c r="E4" s="30"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="17" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="33"/>
-      <c r="H5" s="18" t="s">
+      <c r="E5" s="32"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1353,7 +1482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1361,7 +1490,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1370,7 +1499,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1379,7 +1508,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1388,7 +1517,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1397,7 +1526,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1406,7 +1535,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1415,7 +1544,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1424,7 +1553,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1433,7 +1562,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1442,7 +1571,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1451,7 +1580,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1460,7 +1589,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1469,7 +1598,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1478,7 +1607,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1487,7 +1616,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1496,7 +1625,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1505,7 +1634,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1514,7 +1643,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1523,7 +1652,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1532,7 +1661,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1541,14 +1670,11 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="12" t="s">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="13"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="1"/>
     </row>
   </sheetData>
@@ -1566,7 +1692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1576,86 +1702,86 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.89453125" style="6"/>
-    <col min="2" max="2" width="12.3125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.3125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.9453125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.62890625" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.89453125" style="6"/>
-    <col min="9" max="9" width="26.734375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.89453125" style="6"/>
+    <col min="5" max="5" width="24" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="24" t="s">
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
       <c r="H2" s="3"/>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="H3" s="18" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="17" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="H4" s="18" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="H5" s="18" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1672,7 +1798,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1681,7 +1807,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1691,7 +1817,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1701,7 +1827,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1711,7 +1837,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1721,7 +1847,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1731,7 +1857,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1741,7 +1867,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1751,7 +1877,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1761,7 +1887,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1771,7 +1897,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1781,7 +1907,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1791,7 +1917,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1801,7 +1927,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1811,7 +1937,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1821,7 +1947,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1831,7 +1957,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1841,7 +1967,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1851,7 +1977,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1861,7 +1987,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1871,7 +1997,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1881,16 +2007,13 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="C32" s="34" t="s">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="19"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
review report - coding phase
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Anul3Sem2\ValidareaVerificareaSistemlorSoft\Labs\Grupul_Angajatilor_Young\Docs\Lab1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\Semestrul6\VVSS\labs\Grupul_Angajatilor_Young\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE53C4A-EF5D-49A8-89D3-2E747674BFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93F0005-6F1D-4026-913C-D765AFE4E8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="852" windowWidth="23004" windowHeight="11508" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -18,25 +18,12 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="Tool-basedCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -360,18 +347,79 @@
         this.totalAmount = totalAmount;
     }</t>
   </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>Cantitatea pizzei se seteaza dupa adaugarea pizzei la comanda - se selecteaza pizza, se apasa 'Add to order', apoi se selecteaza din combobox cantitatea, in loc sa se adauge la comanda cantitatea selectata din combobox la apasarea pe 'Add to order'</t>
+  </si>
+  <si>
+    <t>La apasarea butonului de gatire a comenzii (Cook), nu se verifica daca o comanda din lista a fost selectata</t>
+  </si>
+  <si>
+    <t>KitchenGUIController.java - linia 50</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java - linia 136</t>
+  </si>
+  <si>
+    <t>Se face plata chiar daca pretul comenzii este 0</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java - linia 95</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -577,83 +625,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,19 +1067,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1054,10 +1103,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1072,10 +1121,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="28"/>
+      <c r="E5" s="29"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1087,15 +1136,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1290,7 +1339,7 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D5:E5"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1304,7 +1353,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1323,19 +1372,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1359,10 +1408,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="29" t="s">
+      <c r="D4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="29"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1377,10 +1426,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="31"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1392,15 +1441,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1614,7 +1663,7 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D5:E5"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1627,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1648,19 +1697,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1673,31 +1722,39 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="I3" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="J3" s="17">
+        <v>232</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3">
+        <v>232</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1709,15 +1766,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1733,20 +1790,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
@@ -1755,7 +1820,9 @@
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
@@ -1764,7 +1831,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
@@ -1773,43 +1842,61 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
@@ -1818,7 +1905,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
@@ -1827,7 +1916,9 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
@@ -1836,7 +1927,9 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
@@ -1937,6 +2030,7 @@
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="D5:E5"/>
   </mergeCells>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1949,7 +2043,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -1971,19 +2065,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2007,10 +2101,10 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2023,8 +2117,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2036,8 +2130,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2057,7 +2151,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2088,7 +2182,7 @@
       <c r="E11" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="23" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2119,7 +2213,7 @@
       <c r="D13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="37" t="s">
+      <c r="E13" s="23" t="s">
         <v>75</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -2325,11 +2419,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="D32" s="37"/>
+      <c r="E32" s="37"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed code to fix identified coding defects
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\Semestrul6\VVSS\labs\Grupul_Angajatilor_Young\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93F0005-6F1D-4026-913C-D765AFE4E8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D79CC4-C000-4C4F-9229-0ED080742C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -393,13 +393,13 @@
     <t>KitchenGUIController.java - linia 50</t>
   </si>
   <si>
-    <t>OrdersGUIController.java - linia 136</t>
-  </si>
-  <si>
     <t>Se face plata chiar daca pretul comenzii este 0</t>
   </si>
   <si>
-    <t>OrdersGUIController.java - linia 95</t>
+    <t>OrdersGUIController.java - linia 99</t>
+  </si>
+  <si>
+    <t>OrdersGUIController.java - linia 140</t>
   </si>
 </sst>
 </file>
@@ -660,6 +660,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -702,7 +703,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,19 +1067,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1103,10 +1103,10 @@
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1121,10 +1121,10 @@
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1136,15 +1136,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1372,19 +1372,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1408,10 +1408,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -1426,10 +1426,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1441,15 +1441,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1676,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1697,19 +1697,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -1722,7 +1722,7 @@
       <c r="H3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="24" t="s">
         <v>43</v>
       </c>
       <c r="J3" s="17">
@@ -1733,14 +1733,14 @@
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="38" t="s">
+      <c r="I4" s="24" t="s">
         <v>44</v>
       </c>
       <c r="J4" s="3">
@@ -1751,10 +1751,10 @@
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -1766,15 +1766,15 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
@@ -1798,7 +1798,7 @@
         <v>90</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>102</v>
@@ -1857,10 +1857,10 @@
         <v>95</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2065,19 +2065,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="19" t="s">
         <v>30</v>
@@ -2101,10 +2101,10 @@
       <c r="C4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
         <v>21</v>
       </c>
@@ -2117,8 +2117,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
       <c r="H5" s="17" t="s">
         <v>22</v>
       </c>
@@ -2130,8 +2130,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2419,11 +2419,11 @@
       <c r="F30" s="2"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="36" t="s">
+      <c r="C32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="18"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed code to match sonarlint analysis
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\Semestrul6\VVSS\labs\Grupul_Angajatilor_Young\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D79CC4-C000-4C4F-9229-0ED080742C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D59A2C2-416F-4813-92E2-45CE4C372BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -218,9 +218,6 @@
   </si>
   <si>
     <t>public void initGUI()</t>
-  </si>
-  <si>
-    <t>PyamentAlert:18</t>
   </si>
   <si>
     <t xml:space="preserve">String literal should not be duplicated </t>
@@ -400,6 +397,14 @@
   </si>
   <si>
     <t>OrdersGUIController.java - linia 140</t>
+  </si>
+  <si>
+    <t>PaymentAlert:18</t>
+  </si>
+  <si>
+    <t>public void setTotalAmount(double totalAmount) {
+        OrdersGUIController.totalAmount = totalAmount;
+    }</t>
   </si>
 </sst>
 </file>
@@ -1676,7 +1681,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
@@ -1795,13 +1800,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1810,7 +1815,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
@@ -1821,7 +1826,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
@@ -1832,7 +1837,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1843,7 +1848,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1854,13 +1859,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1869,7 +1874,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1880,13 +1885,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1895,7 +1900,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1906,7 +1911,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
@@ -1917,7 +1922,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1928,7 +1933,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
@@ -2043,8 +2048,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2174,16 +2179,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="23" t="s">
         <v>67</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2192,14 +2197,14 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2208,16 +2213,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="F13" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2226,16 +2231,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="F14" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2244,16 +2249,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2262,14 +2267,14 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -2278,15 +2283,17 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">

</xml_diff>

<commit_message>
lab2 - junit tests + BBT_TCs_Form
</commit_message>
<xml_diff>
--- a/Docs/Lab1/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab1/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\Semestrul6\VVSS\labs\Grupul_Angajatilor_Young\Docs\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D59A2C2-416F-4813-92E2-45CE4C372BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B13FE7-FF18-4975-85BF-B959B5B9AD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="110">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -190,19 +190,10 @@
     <t>A10</t>
   </si>
   <si>
-    <t xml:space="preserve">Arhitectura Stratificata </t>
-  </si>
-  <si>
     <t>Yes - Observer. Atunci cand se plaseaza un order apare pe fereastra bucatarului</t>
   </si>
   <si>
-    <t>Nu exista vreun sistem de erori personalizat.</t>
-  </si>
-  <si>
     <t>Da - MainGui - OrderGui - KitchenGui</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80% - avem Payment, PaymentType, dar Meniul si Comanda nu sunt decuplate </t>
   </si>
   <si>
     <t>SonarLint</t>
@@ -405,6 +396,18 @@
     <t>public void setTotalAmount(double totalAmount) {
         OrdersGUIController.totalAmount = totalAmount;
     }</t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>Nu, PaymentAlert era in pachetul de Service, dar lucreaza la interfata, deci trebuie sa fie in pachetul de GUI</t>
+  </si>
+  <si>
+    <t>Nu exista vreun sistem de erori personalizat. Am adaugat PizzaException</t>
+  </si>
+  <si>
+    <t>PizzaService facea si salvare de plati si afisare de menu, am inlocuit cu doua service-uri</t>
   </si>
 </sst>
 </file>
@@ -1357,8 +1360,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,7 +1483,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1490,7 +1493,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1515,7 +1518,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1525,7 +1528,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -1538,7 +1541,7 @@
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1551,10 +1554,10 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1563,7 +1566,9 @@
         <v>52</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
@@ -1576,7 +1581,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1586,7 +1591,7 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>59</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -1681,8 +1686,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1800,13 +1805,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1815,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
@@ -1826,7 +1831,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
@@ -1837,7 +1842,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1848,7 +1853,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1859,13 +1864,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1874,7 +1879,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1885,13 +1890,13 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1900,7 +1905,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1911,7 +1916,7 @@
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
@@ -1922,7 +1927,7 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1933,7 +1938,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
@@ -2048,8 +2053,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2107,7 +2112,7 @@
         <v>25</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E4" s="34"/>
       <c r="H4" s="17" t="s">
@@ -2161,16 +2166,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2179,16 +2184,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2197,14 +2202,14 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2213,16 +2218,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2231,16 +2236,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2249,16 +2254,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2267,14 +2272,14 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="115.2" x14ac:dyDescent="0.3">
@@ -2283,16 +2288,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>